<commit_message>
update click customer và status product và delete sku
</commit_message>
<xml_diff>
--- a/tests/DesignOrder.xlsx
+++ b/tests/DesignOrder.xlsx
@@ -403,7 +403,7 @@
   </sheetViews>
   <cols>
     <col min="1" max="1" customWidth="1" width="13"/>
-    <col min="2" max="2" customWidth="1" width="56"/>
+    <col min="2" max="2" customWidth="1" width="57"/>
     <col min="3" max="3" customWidth="1" width="11"/>
     <col min="4" max="4" customWidth="1" width="8"/>
     <col min="5" max="5" customWidth="1" width="19"/>
@@ -556,10 +556,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>#1415</v>
+        <v>#1429</v>
       </c>
       <c r="B2" t="str">
-        <v>A Product Support Excel T-shirt 2D lần 3 0310 - Black</v>
+        <v>A Product Support Excel T-shirt 2D lần 15 0310 - Black</v>
       </c>
       <c r="C2" t="str">
         <v>3</v>
@@ -568,7 +568,7 @@
         <v>225</v>
       </c>
       <c r="E2" t="str">
-        <v>03:35 03/10/2024</v>
+        <v>05:21 03/10/2024</v>
       </c>
       <c r="F2" t="str">
         <v>THF-S25</v>
@@ -577,10 +577,10 @@
         <v>sale_UyenThu</v>
       </c>
       <c r="H2" t="str">
-        <v>luyenstore_6450889326664</v>
+        <v>luyenstore_6450966757448</v>
       </c>
       <c r="I2" t="str">
-        <v>40416853950536</v>
+        <v>40416861683784</v>
       </c>
       <c r="J2" t="str">
         <v>10</v>
@@ -601,7 +601,7 @@
         <v>0</v>
       </c>
       <c r="P2" t="str">
-        <v>https://cdn.shopify.com/s/files/1/0013/7602/6696/files/c9d00636ce2b818b96e07fa5087aa300_69311d4b-eddd-4ae6-8246-b91bddedf2be.jpg?v=1727944470</v>
+        <v>https://cdn.shopify.com/s/files/1/0013/7602/6696/files/c9d00636ce2b818b96e07fa5087aa300_3f44b37b-66a1-4375-94c8-21357320a95e.jpg?v=1727950833</v>
       </c>
       <c r="Q2" t="str">
         <v>Black</v>

</xml_diff>